<commit_message>
finished integration frequency but bugs remain with some segs having freq na
</commit_message>
<xml_diff>
--- a/segments.xlsx
+++ b/segments.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="460" windowWidth="17100" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="2540" yWindow="460" windowWidth="20640" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="segments.txt" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">segments.txt!$A$1:$G$61</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="166">
   <si>
     <t>:ii</t>
   </si>
@@ -519,13 +519,19 @@
   </si>
   <si>
     <t>not looked up since not in stimuli</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>ə:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,6 +558,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -574,12 +585,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -858,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1226,7 +1238,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1247,7 +1259,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1261,16 +1273,13 @@
         <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" t="s">
-        <v>162</v>
-      </c>
-      <c r="G16" t="s">
-        <v>162</v>
-      </c>
-      <c r="H16" t="s">
-        <v>163</v>
+        <v>134</v>
+      </c>
+      <c r="F16" s="5">
+        <v>104</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2390,13 +2399,36 @@
         <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="F61">
         <v>1003</v>
       </c>
       <c r="G61">
         <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" t="s">
+        <v>89</v>
+      </c>
+      <c r="F62">
+        <v>2483</v>
+      </c>
+      <c r="G62">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
phone frequency extracted but not yet integrated
</commit_message>
<xml_diff>
--- a/segments.xlsx
+++ b/segments.xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acristia/Documents/gitrepos/nwryd19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandrinacristia/gitrepos/nwryd19/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="460" windowWidth="20640" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="15740" yWindow="3380" windowWidth="20640" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="segments.txt" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">segments.txt!$A$1:$G$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">segments.txt!$A$1:$I$62</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="166">
   <si>
     <t>:ii</t>
   </si>
@@ -870,18 +870,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="168" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="168" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -907,7 +909,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -932,8 +934,11 @@
       <c r="H2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -958,62 +963,65 @@
       <c r="H3" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
         <v>134</v>
       </c>
       <c r="F4">
-        <v>223</v>
+        <v>46</v>
       </c>
       <c r="G4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
         <v>134</v>
       </c>
       <c r="F5">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
+        <v>94</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>86</v>
@@ -1022,13 +1030,13 @@
         <v>134</v>
       </c>
       <c r="F6">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1053,8 +1061,11 @@
       <c r="H7" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1079,8 +1090,11 @@
       <c r="H8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1105,8 +1119,11 @@
       <c r="H9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1131,31 +1148,34 @@
       <c r="H10" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" t="s">
-        <v>140</v>
+        <v>93</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
         <v>134</v>
       </c>
       <c r="F11">
-        <v>225</v>
+        <v>20</v>
       </c>
       <c r="G11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1180,8 +1200,11 @@
       <c r="H12" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1206,8 +1229,11 @@
       <c r="H13" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1232,8 +1258,11 @@
       <c r="H14" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1258,54 +1287,57 @@
       <c r="H15" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>138</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="5">
-        <v>104</v>
+      <c r="F16">
+        <v>223</v>
       </c>
       <c r="G16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
         <v>134</v>
       </c>
       <c r="F17">
-        <v>16</v>
+        <v>225</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1330,8 +1362,11 @@
       <c r="H18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1356,16 +1391,19 @@
       <c r="H19" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
+        <v>101</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>87</v>
@@ -1373,60 +1411,66 @@
       <c r="E20" t="s">
         <v>134</v>
       </c>
-      <c r="F20">
-        <v>641</v>
+      <c r="F20" s="5">
+        <v>104</v>
       </c>
       <c r="G20">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
         <v>134</v>
       </c>
       <c r="F21">
-        <v>675</v>
+        <v>707</v>
       </c>
       <c r="G21">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="H21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
+        <v>116</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
         <v>134</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>137</v>
       </c>
@@ -1449,53 +1493,53 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
         <v>134</v>
       </c>
       <c r="F24">
-        <v>436</v>
+        <v>675</v>
       </c>
       <c r="G24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
         <v>134</v>
       </c>
       <c r="F25">
-        <v>2779</v>
+        <v>641</v>
       </c>
       <c r="G25">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -1520,16 +1564,19 @@
       <c r="H26" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
         <v>89</v>
@@ -1538,13 +1585,13 @@
         <v>134</v>
       </c>
       <c r="F27">
-        <v>2716</v>
+        <v>436</v>
       </c>
       <c r="G27">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1569,8 +1616,11 @@
       <c r="H28" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1595,32 +1645,34 @@
       <c r="H29" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E30" t="s">
         <v>134</v>
       </c>
       <c r="F30">
-        <v>373</v>
+        <v>2779</v>
       </c>
       <c r="G30">
-        <v>12</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1645,8 +1697,11 @@
       <c r="H31" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1671,8 +1726,11 @@
       <c r="H32" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1697,8 +1755,11 @@
       <c r="H33" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1723,8 +1784,11 @@
       <c r="H34" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -1749,16 +1813,19 @@
       <c r="H35" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
         <v>89</v>
@@ -1767,24 +1834,22 @@
         <v>134</v>
       </c>
       <c r="F36">
-        <v>10</v>
+        <v>373</v>
       </c>
       <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" t="s">
-        <v>149</v>
+        <v>82</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>89</v>
@@ -1793,21 +1858,24 @@
         <v>134</v>
       </c>
       <c r="F37">
-        <v>2914</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
         <v>89</v>
@@ -1816,16 +1884,13 @@
         <v>134</v>
       </c>
       <c r="F38">
-        <v>532</v>
+        <v>2914</v>
       </c>
       <c r="G38">
-        <v>18</v>
-      </c>
-      <c r="H38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -1850,8 +1915,11 @@
       <c r="H39" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -1876,8 +1944,11 @@
       <c r="H40" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -1902,8 +1973,11 @@
       <c r="H41" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -1928,8 +2002,11 @@
       <c r="H42" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -1954,8 +2031,11 @@
       <c r="H43" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1980,8 +2060,11 @@
       <c r="H44" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2006,8 +2089,11 @@
       <c r="H45" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -2032,8 +2118,11 @@
       <c r="H46" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -2058,8 +2147,11 @@
       <c r="H47" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -2084,8 +2176,11 @@
       <c r="H48" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -2110,8 +2205,11 @@
       <c r="H49" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -2136,8 +2234,11 @@
       <c r="H50" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -2162,8 +2263,11 @@
       <c r="H51" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -2188,8 +2292,11 @@
       <c r="H52" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -2214,62 +2321,68 @@
       <c r="H53" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>106</v>
+        <v>115</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="E54" t="s">
         <v>134</v>
       </c>
       <c r="F54">
-        <v>1070</v>
+        <v>532</v>
       </c>
       <c r="G54">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H54" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>150</v>
-      </c>
-      <c r="B55" t="s">
-        <v>150</v>
+        <v>142</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E55" t="s">
         <v>134</v>
       </c>
       <c r="F55">
-        <v>2594</v>
+        <v>1070</v>
       </c>
       <c r="G55">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>153</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="B56" t="s">
+        <v>150</v>
       </c>
       <c r="C56" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D56" t="s">
         <v>89</v>
@@ -2278,21 +2391,21 @@
         <v>134</v>
       </c>
       <c r="F56">
-        <v>2064</v>
+        <v>2594</v>
       </c>
       <c r="G56">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D57" t="s">
         <v>89</v>
@@ -2301,16 +2414,13 @@
         <v>134</v>
       </c>
       <c r="F57">
-        <v>707</v>
+        <v>2064</v>
       </c>
       <c r="G57">
-        <v>23</v>
-      </c>
-      <c r="H57" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2336,105 +2446,110 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E59" t="s">
         <v>134</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>2646</v>
       </c>
       <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>13</v>
       </c>
       <c r="D60" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="E60" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60">
+        <v>1003</v>
+      </c>
+      <c r="G60">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" t="s">
+        <v>89</v>
+      </c>
+      <c r="F61">
+        <v>2483</v>
+      </c>
+      <c r="G61">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>151</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" t="s">
         <v>134</v>
       </c>
-      <c r="F60">
-        <v>2646</v>
-      </c>
-      <c r="G60">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>52</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" t="s">
-        <v>87</v>
-      </c>
-      <c r="E61" t="s">
-        <v>89</v>
-      </c>
-      <c r="F61">
-        <v>1003</v>
-      </c>
-      <c r="G61">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>164</v>
-      </c>
-      <c r="B62" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E62" t="s">
-        <v>89</v>
-      </c>
       <c r="F62">
-        <v>2483</v>
+        <v>2716</v>
       </c>
       <c r="G62">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G61">
-    <sortState ref="A4:G61">
-      <sortCondition ref="B1:B61"/>
+  <autoFilter ref="A1:I62">
+    <filterColumn colId="7">
+      <filters blank="1">
+        <filter val="AC interpreted dot as dental, so looked up dental n (not advanced n)"/>
+        <filter val="AC interpreted dot as dental, so looked up dental t (not advanced t)"/>
+        <filter val="AC used pt"/>
+        <filter val="AC used βʲ so this may be an overestimate"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A4:I62">
+      <sortCondition ref="A1:A62"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>